<commit_message>
Config scrolls, AB and curve distances
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="121">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -371,6 +371,24 @@
   </si>
   <si>
     <t>EC</t>
+  </si>
+  <si>
+    <t>Tool Steering</t>
+  </si>
+  <si>
+    <t>EB</t>
+  </si>
+  <si>
+    <t>Low XTE</t>
+  </si>
+  <si>
+    <t>High XTE</t>
+  </si>
+  <si>
+    <t>Low Veh XTE</t>
+  </si>
+  <si>
+    <t>High Veh XTE</t>
   </si>
 </sst>
 </file>
@@ -794,6 +812,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,21 +840,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1130,7 +1148,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1141,7 +1159,7 @@
   <dimension ref="A1:AD66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1156,15 +1174,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1285,17 +1303,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="54"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="56"/>
+      <c r="J5" s="61"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1343,18 +1361,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58" t="s">
+      <c r="G7" s="53"/>
+      <c r="H7" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58" t="s">
+      <c r="I7" s="53"/>
+      <c r="J7" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="58"/>
+      <c r="K7" s="53"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1413,10 +1431,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="58"/>
+      <c r="L9" s="53"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1716,34 +1734,34 @@
       <c r="E20" s="22">
         <v>24</v>
       </c>
-      <c r="F20" s="61">
+      <c r="F20" s="52">
         <v>1</v>
       </c>
-      <c r="G20" s="61">
+      <c r="G20" s="52">
         <v>2</v>
       </c>
-      <c r="H20" s="61">
+      <c r="H20" s="52">
         <v>3</v>
       </c>
-      <c r="I20" s="61">
+      <c r="I20" s="52">
         <v>4</v>
       </c>
-      <c r="J20" s="61">
+      <c r="J20" s="52">
         <v>5</v>
       </c>
-      <c r="K20" s="61">
+      <c r="K20" s="52">
         <v>6</v>
       </c>
-      <c r="L20" s="61">
+      <c r="L20" s="52">
         <v>7</v>
       </c>
-      <c r="M20" s="61">
+      <c r="M20" s="52">
         <v>8</v>
       </c>
-      <c r="N20" s="61">
+      <c r="N20" s="52">
         <v>9</v>
       </c>
-      <c r="O20" s="61">
+      <c r="O20" s="52">
         <v>10</v>
       </c>
       <c r="P20" s="2">
@@ -1808,18 +1826,46 @@
       <c r="O21" s="44"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A22" s="34" t="s">
+        <v>115</v>
+      </c>
       <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
+      <c r="C22" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="43">
+        <v>235</v>
+      </c>
+      <c r="E22" s="22">
+        <v>8</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="K22" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="M22" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="N22" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="O22" s="44"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
@@ -2059,18 +2105,18 @@
       <c r="E33" s="46">
         <v>8</v>
       </c>
-      <c r="F33" s="59" t="s">
+      <c r="F33" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60" t="s">
+      <c r="G33" s="55"/>
+      <c r="H33" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="I33" s="60"/>
-      <c r="J33" s="58" t="s">
+      <c r="I33" s="55"/>
+      <c r="J33" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="K33" s="58"/>
+      <c r="K33" s="53"/>
       <c r="L33" s="44">
         <v>0</v>
       </c>
@@ -2151,14 +2197,14 @@
         <f>HEX2DEC(C37)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2185,14 +2231,14 @@
         <v>87</v>
       </c>
       <c r="D39" s="43"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
       <c r="N39" s="44"/>
       <c r="O39" s="44"/>
     </row>
@@ -2539,6 +2585,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="F33:G33"/>
     <mergeCell ref="H33:I33"/>
@@ -2546,12 +2598,6 @@
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="J39:M39"/>
     <mergeCell ref="J33:K33"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2716,15 +2762,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2888,6 +2925,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2895,14 +2941,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2920,6 +2958,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
new tool form steering
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="123">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>High Veh XTE</t>
+  </si>
+  <si>
+    <t>ToolConfig</t>
+  </si>
+  <si>
+    <t>Tool Settings</t>
   </si>
 </sst>
 </file>
@@ -667,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -818,28 +824,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1148,7 +1160,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1156,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD66"/>
+  <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1174,15 +1186,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1303,17 +1315,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="59"/>
+      <c r="G5" s="57"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="61"/>
+      <c r="J5" s="59"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1361,18 +1373,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53" t="s">
+      <c r="G7" s="61"/>
+      <c r="H7" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53" t="s">
+      <c r="I7" s="61"/>
+      <c r="J7" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="53"/>
+      <c r="K7" s="61"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1431,10 +1443,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="53" t="s">
+      <c r="K9" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="53"/>
+      <c r="L9" s="61"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1941,191 +1953,176 @@
       <c r="O25" s="44"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="44"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="44"/>
-      <c r="N26" s="44"/>
-      <c r="O26" s="44"/>
+      <c r="A26" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54">
+        <v>233</v>
+      </c>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="44"/>
-    </row>
-    <row r="28" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="35"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="38"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-    </row>
-    <row r="29" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A28" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43">
+        <v>232</v>
+      </c>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+    </row>
+    <row r="30" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="35"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="39"/>
+    </row>
+    <row r="31" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B31" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C31" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="46">
+      <c r="D31" s="46">
         <v>214</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E31" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="47"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
-      <c r="O29" s="47"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-      <c r="R29" s="48"/>
-    </row>
-    <row r="30" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="45"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-      <c r="R30" s="48"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="43">
-        <v>212</v>
-      </c>
-      <c r="E31" s="22">
-        <v>2</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+    </row>
+    <row r="32" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="45"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="48"/>
+      <c r="R32" s="48"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D33" s="43">
-        <f>HEX2DEC(C33)</f>
-        <v>211</v>
-      </c>
-      <c r="E33" s="46">
-        <v>8</v>
-      </c>
-      <c r="F33" s="54" t="s">
-        <v>82</v>
-      </c>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="55"/>
-      <c r="J33" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="K33" s="53"/>
-      <c r="L33" s="44">
-        <v>0</v>
-      </c>
-      <c r="M33" s="44">
-        <v>0</v>
-      </c>
-      <c r="N33" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" s="22">
+        <v>2</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" s="44" t="s">
         <v>27</v>
       </c>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
       <c r="O33" s="44"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -2145,32 +2142,42 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="34" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C35" s="43" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D35" s="43">
         <f>HEX2DEC(C35)</f>
-        <v>210</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
+        <v>211</v>
+      </c>
+      <c r="E35" s="46">
+        <v>8</v>
+      </c>
+      <c r="F35" s="62" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" s="63"/>
+      <c r="H35" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" s="63"/>
+      <c r="J35" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="K35" s="61"/>
+      <c r="L35" s="44">
+        <v>0</v>
+      </c>
+      <c r="M35" s="44">
+        <v>0</v>
+      </c>
+      <c r="N35" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="O35" s="44"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -2189,22 +2196,32 @@
       <c r="O36" s="44"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="34" t="s">
+        <v>84</v>
+      </c>
       <c r="B37" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="43"/>
+      <c r="C37" s="43" t="s">
+        <v>85</v>
+      </c>
       <c r="D37" s="43">
         <f>HEX2DEC(C37)</f>
-        <v>0</v>
-      </c>
-      <c r="F37" s="53"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="53"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
+        <v>210</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
       <c r="N37" s="44"/>
       <c r="O37" s="44"/>
     </row>
@@ -2227,18 +2244,19 @@
       <c r="B39" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="43"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="53"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43">
+        <f>HEX2DEC(C39)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
       <c r="N39" s="44"/>
       <c r="O39" s="44"/>
     </row>
@@ -2258,28 +2276,21 @@
       <c r="O40" s="44"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="34" t="s">
-        <v>101</v>
-      </c>
       <c r="B41" s="43" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D41" s="43"/>
-      <c r="F41" s="44">
-        <v>1</v>
-      </c>
-      <c r="G41" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="44"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="44"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+      <c r="L41" s="61"/>
+      <c r="M41" s="61"/>
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
     </row>
@@ -2299,11 +2310,22 @@
       <c r="O42" s="44"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
+      <c r="A43" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>100</v>
+      </c>
       <c r="D43" s="43"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
+      <c r="F43" s="44">
+        <v>1</v>
+      </c>
+      <c r="G43" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="H43" s="44"/>
       <c r="I43" s="44"/>
       <c r="J43" s="44"/>
@@ -2312,6 +2334,21 @@
       <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="44"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+      <c r="O44" s="44"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B45" s="43"/>
@@ -2358,21 +2395,6 @@
       <c r="N49" s="44"/>
       <c r="O49" s="44"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-      <c r="J50" s="44"/>
-      <c r="K50" s="44"/>
-      <c r="L50" s="44"/>
-      <c r="M50" s="44"/>
-      <c r="N50" s="44"/>
-      <c r="O50" s="44"/>
-    </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
@@ -2418,6 +2440,21 @@
       <c r="N53" s="44"/>
       <c r="O53" s="44"/>
     </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B54" s="43"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="44"/>
+      <c r="L54" s="44"/>
+      <c r="M54" s="44"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="44"/>
+    </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
@@ -2448,21 +2485,6 @@
       <c r="N57" s="44"/>
       <c r="O57" s="44"/>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B58" s="43"/>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="44"/>
-      <c r="I58" s="44"/>
-      <c r="J58" s="44"/>
-      <c r="K58" s="44"/>
-      <c r="L58" s="44"/>
-      <c r="M58" s="44"/>
-      <c r="N58" s="44"/>
-      <c r="O58" s="44"/>
-    </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B59" s="43"/>
       <c r="C59" s="43"/>
@@ -2583,21 +2605,51 @@
       <c r="N66" s="44"/>
       <c r="O66" s="44"/>
     </row>
+    <row r="67" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B67" s="43"/>
+      <c r="C67" s="43"/>
+      <c r="D67" s="43"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="44"/>
+      <c r="I67" s="44"/>
+      <c r="J67" s="44"/>
+      <c r="K67" s="44"/>
+      <c r="L67" s="44"/>
+      <c r="M67" s="44"/>
+      <c r="N67" s="44"/>
+      <c r="O67" s="44"/>
+    </row>
+    <row r="68" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B68" s="43"/>
+      <c r="C68" s="43"/>
+      <c r="D68" s="43"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="44"/>
+      <c r="H68" s="44"/>
+      <c r="I68" s="44"/>
+      <c r="J68" s="44"/>
+      <c r="K68" s="44"/>
+      <c r="L68" s="44"/>
+      <c r="M68" s="44"/>
+      <c r="N68" s="44"/>
+      <c r="O68" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="F39:M39"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J35:K35"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="F37:M37"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J33:K33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2762,6 +2814,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2925,15 +2986,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2941,6 +2993,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2958,14 +3018,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
AgIO and Machine Steer UDP
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>Tool Settings</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>From Machine</t>
   </si>
 </sst>
 </file>
@@ -673,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -830,6 +836,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -840,18 +864,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1160,7 +1172,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1168,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD68"/>
+  <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1186,15 +1198,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1315,17 +1327,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="57"/>
+      <c r="G5" s="63"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="59"/>
+      <c r="J5" s="65"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1376,15 +1388,15 @@
       <c r="F7" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61" t="s">
+      <c r="G7" s="57"/>
+      <c r="H7" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61" t="s">
+      <c r="I7" s="57"/>
+      <c r="J7" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="61"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1443,10 +1455,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="61" t="s">
+      <c r="K9" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="61"/>
+      <c r="L9" s="57"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1733,152 +1745,144 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="43">
-        <f t="shared" ref="D20" si="0">HEX2DEC(C20)</f>
-        <v>236</v>
+        <v>124</v>
+      </c>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="55">
+        <v>237</v>
       </c>
       <c r="E20" s="22">
-        <v>24</v>
-      </c>
-      <c r="F20" s="52">
+        <v>8</v>
+      </c>
+      <c r="F20" s="56">
         <v>1</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="56">
         <v>2</v>
       </c>
-      <c r="H20" s="52">
+      <c r="H20" s="56">
         <v>3</v>
       </c>
-      <c r="I20" s="52">
+      <c r="I20" s="56">
         <v>4</v>
       </c>
-      <c r="J20" s="52">
-        <v>5</v>
-      </c>
-      <c r="K20" s="52">
-        <v>6</v>
-      </c>
-      <c r="L20" s="52">
-        <v>7</v>
-      </c>
-      <c r="M20" s="52">
-        <v>8</v>
-      </c>
-      <c r="N20" s="52">
-        <v>9</v>
-      </c>
-      <c r="O20" s="52">
-        <v>10</v>
-      </c>
-      <c r="P20" s="2">
-        <v>11</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>12</v>
-      </c>
-      <c r="R20" s="2">
-        <v>13</v>
-      </c>
-      <c r="S20" s="3">
-        <v>14</v>
-      </c>
-      <c r="T20" s="3">
-        <v>15</v>
-      </c>
-      <c r="U20" s="3">
-        <v>16</v>
-      </c>
-      <c r="V20" s="3">
-        <v>17</v>
-      </c>
-      <c r="W20" s="3">
-        <v>18</v>
-      </c>
-      <c r="X20" s="3">
-        <v>19</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>20</v>
-      </c>
-      <c r="Z20" s="3">
-        <v>21</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>22</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>23</v>
-      </c>
-      <c r="AC20" s="3">
-        <v>24</v>
-      </c>
-      <c r="AD20" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="J20" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
-      <c r="N21" s="44"/>
-      <c r="O21" s="44"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B22" s="43"/>
       <c r="C22" s="43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D22" s="43">
-        <v>235</v>
+        <f t="shared" ref="D22" si="0">HEX2DEC(C22)</f>
+        <v>236</v>
       </c>
       <c r="E22" s="22">
+        <v>24</v>
+      </c>
+      <c r="F22" s="52">
+        <v>1</v>
+      </c>
+      <c r="G22" s="52">
+        <v>2</v>
+      </c>
+      <c r="H22" s="52">
+        <v>3</v>
+      </c>
+      <c r="I22" s="52">
+        <v>4</v>
+      </c>
+      <c r="J22" s="52">
+        <v>5</v>
+      </c>
+      <c r="K22" s="52">
+        <v>6</v>
+      </c>
+      <c r="L22" s="52">
+        <v>7</v>
+      </c>
+      <c r="M22" s="52">
         <v>8</v>
       </c>
-      <c r="F22" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="44" t="s">
+      <c r="N22" s="52">
+        <v>9</v>
+      </c>
+      <c r="O22" s="52">
+        <v>10</v>
+      </c>
+      <c r="P22" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>12</v>
+      </c>
+      <c r="R22" s="2">
+        <v>13</v>
+      </c>
+      <c r="S22" s="3">
+        <v>14</v>
+      </c>
+      <c r="T22" s="3">
+        <v>15</v>
+      </c>
+      <c r="U22" s="3">
+        <v>16</v>
+      </c>
+      <c r="V22" s="3">
+        <v>17</v>
+      </c>
+      <c r="W22" s="3">
+        <v>18</v>
+      </c>
+      <c r="X22" s="3">
+        <v>19</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>20</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>21</v>
+      </c>
+      <c r="AA22" s="3">
         <v>22</v>
       </c>
-      <c r="I22" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="K22" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="L22" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="M22" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N22" s="44" t="s">
+      <c r="AB22" s="3">
+        <v>23</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>24</v>
+      </c>
+      <c r="AD22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O22" s="44"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B23" s="43"/>
@@ -1897,45 +1901,46 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>62</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B24" s="43"/>
       <c r="C24" s="43" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="D24" s="43">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="E24" s="22">
+        <v>8</v>
       </c>
       <c r="F24" s="44" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="G24" s="44" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="H24" s="44" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="I24" s="44" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="J24" s="44" t="s">
-        <v>67</v>
+        <v>120</v>
       </c>
       <c r="K24" s="44" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="L24" s="44" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
       <c r="M24" s="44" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="N24" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="O24" s="3"/>
+      <c r="O24" s="44"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B25" s="43"/>
@@ -1954,233 +1959,235 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54">
-        <v>233</v>
-      </c>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
+        <v>61</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="43">
+        <v>234</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="K26" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="M26" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="53"/>
-      <c r="L27" s="53"/>
-      <c r="M27" s="53"/>
-      <c r="N27" s="53"/>
-      <c r="O27" s="53"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54">
+        <v>233</v>
+      </c>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="53"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A30" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43">
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43">
         <v>232</v>
       </c>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-    </row>
-    <row r="30" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="38"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-    </row>
-    <row r="31" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="45" t="s">
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+    </row>
+    <row r="32" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="35"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+    </row>
+    <row r="33" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B33" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="46" t="s">
+      <c r="C33" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="46">
+      <c r="D33" s="46">
         <v>214</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E33" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
-      <c r="K31" s="47"/>
-      <c r="L31" s="47"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-      <c r="R31" s="48"/>
-    </row>
-    <row r="32" spans="1:30" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="45"/>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
-      <c r="R32" s="48"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="34" t="s">
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+      <c r="P33" s="48"/>
+      <c r="Q33" s="48"/>
+      <c r="R33" s="48"/>
+    </row>
+    <row r="34" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="48"/>
+      <c r="Q34" s="48"/>
+      <c r="R34" s="48"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A35" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B35" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="43" t="s">
+      <c r="C35" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="43">
+      <c r="D35" s="43">
         <v>212</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E35" s="22">
         <v>2</v>
       </c>
-      <c r="F33" s="44" t="s">
+      <c r="F35" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="G33" s="44" t="s">
+      <c r="G35" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="44" t="s">
+      <c r="H35" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="44"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="44"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="44"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="44"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="43">
-        <f>HEX2DEC(C35)</f>
-        <v>211</v>
-      </c>
-      <c r="E35" s="46">
-        <v>8</v>
-      </c>
-      <c r="F35" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="G35" s="63"/>
-      <c r="H35" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="I35" s="63"/>
-      <c r="J35" s="61" t="s">
-        <v>98</v>
-      </c>
-      <c r="K35" s="61"/>
-      <c r="L35" s="44">
-        <v>0</v>
-      </c>
-      <c r="M35" s="44">
-        <v>0</v>
-      </c>
-      <c r="N35" s="44" t="s">
-        <v>27</v>
-      </c>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
       <c r="O35" s="44"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B36" s="43"/>
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
@@ -2195,37 +2202,47 @@
       <c r="N36" s="44"/>
       <c r="O36" s="44"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="34" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D37" s="43">
         <f>HEX2DEC(C37)</f>
-        <v>210</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F37" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
-      <c r="M37" s="44"/>
-      <c r="N37" s="44"/>
+        <v>211</v>
+      </c>
+      <c r="E37" s="46">
+        <v>8</v>
+      </c>
+      <c r="F37" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="I37" s="59"/>
+      <c r="J37" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="K37" s="57"/>
+      <c r="L37" s="44">
+        <v>0</v>
+      </c>
+      <c r="M37" s="44">
+        <v>0</v>
+      </c>
+      <c r="N37" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="O37" s="44"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B38" s="43"/>
       <c r="C38" s="43"/>
       <c r="D38" s="43"/>
@@ -2240,27 +2257,37 @@
       <c r="N38" s="44"/>
       <c r="O38" s="44"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A39" s="34" t="s">
+        <v>84</v>
+      </c>
       <c r="B39" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="43"/>
+      <c r="C39" s="43" t="s">
+        <v>85</v>
+      </c>
       <c r="D39" s="43">
         <f>HEX2DEC(C39)</f>
-        <v>0</v>
-      </c>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
+        <v>210</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
       <c r="N39" s="44"/>
       <c r="O39" s="44"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
       <c r="D40" s="43"/>
@@ -2275,26 +2302,27 @@
       <c r="N40" s="44"/>
       <c r="O40" s="44"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="43"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="61"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43">
+        <f>HEX2DEC(C41)</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57"/>
+      <c r="M41" s="57"/>
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -2309,33 +2337,26 @@
       <c r="N42" s="44"/>
       <c r="O42" s="44"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="34" t="s">
-        <v>101</v>
-      </c>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B43" s="43" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="D43" s="43"/>
-      <c r="F43" s="44">
-        <v>1</v>
-      </c>
-      <c r="G43" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
       <c r="N43" s="44"/>
       <c r="O43" s="44"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B44" s="43"/>
       <c r="C44" s="43"/>
       <c r="D44" s="43"/>
@@ -2350,12 +2371,23 @@
       <c r="N44" s="44"/>
       <c r="O44" s="44"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A45" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>100</v>
+      </c>
       <c r="D45" s="43"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
+      <c r="F45" s="44">
+        <v>1</v>
+      </c>
+      <c r="G45" s="44" t="s">
+        <v>27</v>
+      </c>
       <c r="H45" s="44"/>
       <c r="I45" s="44"/>
       <c r="J45" s="44"/>
@@ -2365,7 +2397,22 @@
       <c r="N45" s="44"/>
       <c r="O45" s="44"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="44"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
       <c r="D47" s="43"/>
@@ -2410,21 +2457,6 @@
       <c r="N51" s="44"/>
       <c r="O51" s="44"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="44"/>
-      <c r="L52" s="44"/>
-      <c r="M52" s="44"/>
-      <c r="N52" s="44"/>
-      <c r="O52" s="44"/>
-    </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
@@ -2470,6 +2502,21 @@
       <c r="N55" s="44"/>
       <c r="O55" s="44"/>
     </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B56" s="43"/>
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="44"/>
+      <c r="M56" s="44"/>
+      <c r="N56" s="44"/>
+      <c r="O56" s="44"/>
+    </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
@@ -2500,21 +2547,6 @@
       <c r="N59" s="44"/>
       <c r="O59" s="44"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B60" s="43"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="43"/>
-      <c r="F60" s="44"/>
-      <c r="G60" s="44"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="44"/>
-      <c r="K60" s="44"/>
-      <c r="L60" s="44"/>
-      <c r="M60" s="44"/>
-      <c r="N60" s="44"/>
-      <c r="O60" s="44"/>
-    </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B61" s="43"/>
       <c r="C61" s="43"/>
@@ -2635,21 +2667,51 @@
       <c r="N68" s="44"/>
       <c r="O68" s="44"/>
     </row>
+    <row r="69" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B69" s="43"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="44"/>
+      <c r="H69" s="44"/>
+      <c r="I69" s="44"/>
+      <c r="J69" s="44"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="44"/>
+      <c r="M69" s="44"/>
+      <c r="N69" s="44"/>
+      <c r="O69" s="44"/>
+    </row>
+    <row r="70" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B70" s="43"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="44"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="44"/>
+      <c r="K70" s="44"/>
+      <c r="L70" s="44"/>
+      <c r="M70" s="44"/>
+      <c r="N70" s="44"/>
+      <c r="O70" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="F39:M39"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J35:K35"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="F41:M41"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2814,15 +2876,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100168D69F7049F5C4D941A1ED43A3EBF4E" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6358b93c66be89da512ed1b0037fb663">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac7999f6-dd20-429f-9c50-d27a0c8de317" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7603896104695ce44c6e748634a25e45" ns2:_="">
     <xsd:import namespace="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
@@ -2986,6 +3039,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2993,14 +3055,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F34BA2AD-7737-4D5E-9A5C-0001377CDA31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3018,6 +3072,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8B9148-C797-4C6B-A280-0738F64421E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Tool Form and PGN's
</commit_message>
<xml_diff>
--- a/Support/PGN 5.1.xlsx
+++ b/Support/PGN 5.1.xlsx
@@ -10,6 +10,9 @@
     <sheet name="PGN" sheetId="1" r:id="rId1"/>
     <sheet name="fixed IP list" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PGN!$A$1:$N$37</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="143">
   <si>
     <t>Format: 0x80, 0x81, Src, PGN, Length, [Data Bytes], CRC</t>
   </si>
@@ -241,57 +244,12 @@
     <t>Off Group 1</t>
   </si>
   <si>
-    <t>NMEA bytes</t>
-  </si>
-  <si>
-    <t>7C</t>
-  </si>
-  <si>
     <t>D6</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
-    <t>IMU Detach Req</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>Removed</t>
-  </si>
-  <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t>IMU</t>
   </si>
   <si>
-    <t>7D</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>Heading</t>
-  </si>
-  <si>
-    <t>Roll</t>
-  </si>
-  <si>
-    <t>AgIOTraffic</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>Seconds</t>
-  </si>
-  <si>
-    <t>D0</t>
-  </si>
-  <si>
     <t>IP Addresses when using fixed IPs</t>
   </si>
   <si>
@@ -322,9 +280,6 @@
     <t>Tablet Computer</t>
   </si>
   <si>
-    <t>Gyro</t>
-  </si>
-  <si>
     <t xml:space="preserve">7F </t>
   </si>
   <si>
@@ -358,9 +313,6 @@
     <t>FA</t>
   </si>
   <si>
-    <t>valueA0</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -376,9 +328,6 @@
     <t>Tool Steering</t>
   </si>
   <si>
-    <t>EB</t>
-  </si>
-  <si>
     <t>Low XTE</t>
   </si>
   <si>
@@ -401,6 +350,114 @@
   </si>
   <si>
     <t>From Machine</t>
+  </si>
+  <si>
+    <t>Speed * 10</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Integral</t>
+  </si>
+  <si>
+    <t>windup</t>
+  </si>
+  <si>
+    <t>WAS Counts</t>
+  </si>
+  <si>
+    <t>WAS Offset</t>
+  </si>
+  <si>
+    <t>Max Steer</t>
+  </si>
+  <si>
+    <t>Setting 0</t>
+  </si>
+  <si>
+    <t>0=Invert WAS</t>
+  </si>
+  <si>
+    <t>1=Invert Rel</t>
+  </si>
+  <si>
+    <t>2=Inv Steer</t>
+  </si>
+  <si>
+    <t>3=Convertor</t>
+  </si>
+  <si>
+    <t>4=Motor Drv</t>
+  </si>
+  <si>
+    <t>5=Danfoss</t>
+  </si>
+  <si>
+    <t>Bit</t>
+  </si>
+  <si>
+    <t>0=Differential</t>
+  </si>
+  <si>
+    <t>0=IBT2</t>
+  </si>
+  <si>
+    <t>0=off</t>
+  </si>
+  <si>
+    <t>1 = Single</t>
+  </si>
+  <si>
+    <t>1 = Cytron</t>
+  </si>
+  <si>
+    <t>1=on</t>
+  </si>
+  <si>
+    <t>1=inv</t>
+  </si>
+  <si>
+    <t>From  Tool Steer</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>Low Actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Actual </t>
+  </si>
+  <si>
+    <t>Low Error</t>
+  </si>
+  <si>
+    <t>High Error</t>
+  </si>
+  <si>
+    <t>Tool PWM</t>
+  </si>
+  <si>
+    <t>Sensor Value</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>Tool Antenna</t>
+  </si>
+  <si>
+    <t>Main Antenna</t>
   </si>
 </sst>
 </file>
@@ -495,7 +552,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -675,11 +732,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,6 +931,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1180,33 +1305,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD70"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AD75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="34" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="34" customWidth="1"/>
     <col min="2" max="4" width="5.140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="5.140625" style="22" customWidth="1"/>
-    <col min="6" max="15" width="9.85546875" style="1" customWidth="1"/>
+    <col min="6" max="9" width="9.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="1" customWidth="1"/>
+    <col min="11" max="15" width="9.85546875" style="1" customWidth="1"/>
     <col min="16" max="17" width="9.85546875" style="2" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="2"/>
     <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -1327,17 +1457,17 @@
       <c r="E5" s="22">
         <v>8</v>
       </c>
-      <c r="F5" s="62" t="s">
+      <c r="F5" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="74"/>
       <c r="H5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="64" t="s">
+      <c r="I5" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="65"/>
+      <c r="J5" s="76"/>
       <c r="K5" s="44" t="s">
         <v>24</v>
       </c>
@@ -1385,18 +1515,18 @@
       <c r="E7" s="22">
         <v>8</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57" t="s">
+      <c r="G7" s="68"/>
+      <c r="H7" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57" t="s">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="57"/>
+      <c r="K7" s="68"/>
       <c r="L7" s="44" t="s">
         <v>34</v>
       </c>
@@ -1455,10 +1585,10 @@
       <c r="J9" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="K9" s="57" t="s">
+      <c r="K9" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="57"/>
+      <c r="L9" s="68"/>
       <c r="M9" s="44" t="s">
         <v>44</v>
       </c>
@@ -1545,13 +1675,13 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="B13" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="D13" s="50">
         <v>250</v>
@@ -1560,28 +1690,28 @@
         <v>8</v>
       </c>
       <c r="F13" s="51" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="G13" s="51" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="H13" s="51" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="I13" s="51" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="J13" s="51" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="L13" s="51" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="M13" s="51" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="N13" s="51" t="s">
         <v>27</v>
@@ -1644,7 +1774,7 @@
         <v>53</v>
       </c>
       <c r="G16" s="44" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="H16" s="44" t="s">
         <v>54</v>
@@ -1653,7 +1783,7 @@
         <v>55</v>
       </c>
       <c r="J16" s="44" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="K16" s="44" t="s">
         <v>24</v>
@@ -1688,7 +1818,9 @@
       <c r="A18" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="43"/>
+      <c r="B18" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="C18" s="43" t="s">
         <v>57</v>
       </c>
@@ -1712,16 +1844,16 @@
         <v>47</v>
       </c>
       <c r="J18" s="44" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="K18" s="44" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="L18" s="44" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="M18" s="44" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="N18" s="44" t="s">
         <v>27</v>
@@ -1745,11 +1877,13 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="B20" s="55"/>
+        <v>106</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>19</v>
+      </c>
       <c r="C20" s="55" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="D20" s="55">
         <v>237</v>
@@ -1770,7 +1904,7 @@
         <v>4</v>
       </c>
       <c r="J20" s="56" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="K20" s="56"/>
       <c r="L20" s="56"/>
@@ -1795,11 +1929,13 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="43"/>
+        <v>86</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>19</v>
+      </c>
       <c r="C22" s="43" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="D22" s="43">
         <f t="shared" ref="D22" si="0">HEX2DEC(C22)</f>
@@ -1885,144 +2021,145 @@
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="44"/>
-      <c r="N23" s="44"/>
-      <c r="O23" s="44"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24" s="34" t="s">
-        <v>115</v>
-      </c>
       <c r="B24" s="43"/>
-      <c r="C24" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="43">
-        <v>235</v>
-      </c>
-      <c r="E24" s="22">
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+    </row>
+    <row r="25" spans="1:30" s="66" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="63">
+        <v>234</v>
+      </c>
+      <c r="E25" s="64"/>
+      <c r="F25" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="K25" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="N25" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="67"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A27" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="43">
+        <v>233</v>
+      </c>
+      <c r="E27" s="22">
         <v>8</v>
       </c>
-      <c r="F24" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="G24" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="H24" s="44" t="s">
+      <c r="F27" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I24" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="J24" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="K24" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="L24" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="M24" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="N24" s="44" t="s">
+      <c r="I27" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="K27" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="L27" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="M27" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="N27" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="O24" s="44"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="44"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="44"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="43">
-        <v>234</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="J26" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="L26" s="44" t="s">
-        <v>69</v>
-      </c>
-      <c r="M26" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="N26" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="44"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="44"/>
-      <c r="N27" s="44"/>
       <c r="O27" s="44"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54">
-        <v>233</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
       <c r="F28" s="53"/>
       <c r="G28" s="53"/>
       <c r="H28" s="53"/>
@@ -2035,257 +2172,300 @@
       <c r="O28" s="53"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B29" s="54"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="53"/>
-      <c r="M29" s="53"/>
-      <c r="N29" s="53"/>
+      <c r="A29" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="54">
+        <v>232</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="H29" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" s="53" t="s">
+        <v>114</v>
+      </c>
+      <c r="L29" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="M29" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="N29" s="53" t="s">
+        <v>27</v>
+      </c>
       <c r="O29" s="53"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A31" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="43">
+        <v>231</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="H31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="I31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="J31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="L31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="M31" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="N31" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="O31" s="44"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B32" s="58"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="F32" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="H32" s="57" t="s">
+        <v>119</v>
+      </c>
+      <c r="I32" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="J32" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="K32" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43">
-        <v>232</v>
-      </c>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="44"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-    </row>
-    <row r="32" spans="1:30" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="35"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-    </row>
-    <row r="33" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="46">
-        <v>214</v>
-      </c>
-      <c r="E33" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-      <c r="R33" s="48"/>
-    </row>
-    <row r="34" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="45"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="48"/>
-      <c r="R34" s="48"/>
+      <c r="L32" s="57" t="s">
+        <v>123</v>
+      </c>
+      <c r="M32" s="57"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="I34" s="61" t="s">
+        <v>131</v>
+      </c>
+      <c r="J34" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="K34" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="L34" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="43">
-        <v>212</v>
-      </c>
-      <c r="E35" s="22">
-        <v>2</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="G35" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="H35" s="44" t="s">
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A36" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="59">
+        <v>230</v>
+      </c>
+      <c r="F36" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" s="61" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" s="61" t="s">
+        <v>138</v>
+      </c>
+      <c r="K36" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="L36" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="M36" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="N36" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="44"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="44"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="44"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="43">
-        <f>HEX2DEC(C37)</f>
-        <v>211</v>
-      </c>
-      <c r="E37" s="46">
-        <v>8</v>
-      </c>
-      <c r="F37" s="58" t="s">
-        <v>82</v>
-      </c>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="I37" s="59"/>
-      <c r="J37" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="K37" s="57"/>
-      <c r="L37" s="44">
-        <v>0</v>
-      </c>
-      <c r="M37" s="44">
-        <v>0</v>
-      </c>
-      <c r="N37" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="O37" s="44"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="44"/>
-      <c r="O38" s="44"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="43" t="s">
+      <c r="O36" s="60"/>
+    </row>
+    <row r="37" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="35"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+    </row>
+    <row r="38" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="45"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="48"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="48"/>
+    </row>
+    <row r="39" spans="1:18" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="43">
-        <f>HEX2DEC(C39)</f>
-        <v>210</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
-      <c r="O39" s="44"/>
+      <c r="C39" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="46">
+        <v>215</v>
+      </c>
+      <c r="E39" s="22"/>
+      <c r="F39" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="47"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="47"/>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="48"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B40" s="43"/>
@@ -2303,22 +2483,28 @@
       <c r="O40" s="44"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A41" s="34" t="s">
+        <v>142</v>
+      </c>
       <c r="B41" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="43"/>
+      <c r="C41" s="43" t="s">
+        <v>71</v>
+      </c>
       <c r="D41" s="43">
-        <f>HEX2DEC(C41)</f>
-        <v>0</v>
-      </c>
-      <c r="F41" s="57"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="57"/>
-      <c r="J41" s="57"/>
-      <c r="K41" s="57"/>
-      <c r="L41" s="57"/>
-      <c r="M41" s="57"/>
+        <v>214</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
       <c r="N41" s="44"/>
       <c r="O41" s="44"/>
     </row>
@@ -2326,33 +2512,30 @@
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="44"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="70"/>
+      <c r="J42" s="68"/>
+      <c r="K42" s="68"/>
       <c r="L42" s="44"/>
       <c r="M42" s="44"/>
       <c r="N42" s="44"/>
       <c r="O42" s="44"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B43" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="43" t="s">
-        <v>87</v>
-      </c>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
       <c r="D43" s="43"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="57"/>
-      <c r="J43" s="57"/>
-      <c r="K43" s="57"/>
-      <c r="L43" s="57"/>
-      <c r="M43" s="57"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
       <c r="N43" s="44"/>
       <c r="O43" s="44"/>
     </row>
@@ -2372,22 +2555,11 @@
       <c r="O44" s="44"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="B45" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="43" t="s">
-        <v>100</v>
-      </c>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
       <c r="D45" s="43"/>
-      <c r="F45" s="44">
-        <v>1</v>
-      </c>
-      <c r="G45" s="44" t="s">
-        <v>27</v>
-      </c>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
       <c r="H45" s="44"/>
       <c r="I45" s="44"/>
       <c r="J45" s="44"/>
@@ -2401,14 +2573,14 @@
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
       <c r="D46" s="43"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="44"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="68"/>
+      <c r="J46" s="68"/>
+      <c r="K46" s="68"/>
+      <c r="L46" s="68"/>
+      <c r="M46" s="68"/>
       <c r="N46" s="44"/>
       <c r="O46" s="44"/>
     </row>
@@ -2427,9 +2599,31 @@
       <c r="N47" s="44"/>
       <c r="O47" s="44"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="F48" s="71"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="68"/>
+      <c r="I48" s="68"/>
+      <c r="J48" s="68"/>
+      <c r="K48" s="68"/>
+      <c r="L48" s="68"/>
+      <c r="M48" s="68"/>
+      <c r="N48" s="44"/>
+      <c r="O48" s="44"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>84</v>
+      </c>
       <c r="D49" s="43"/>
       <c r="F49" s="44"/>
       <c r="G49" s="44"/>
@@ -2442,7 +2636,22 @@
       <c r="N49" s="44"/>
       <c r="O49" s="44"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B50" s="43"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="44"/>
+      <c r="K50" s="44"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="44"/>
+      <c r="N50" s="44"/>
+      <c r="O50" s="44"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B51" s="43"/>
       <c r="C51" s="43"/>
       <c r="D51" s="43"/>
@@ -2457,25 +2666,24 @@
       <c r="N51" s="44"/>
       <c r="O51" s="44"/>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="44"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="44"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B53" s="43"/>
       <c r="C53" s="43"/>
       <c r="D53" s="43"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="44"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="44"/>
-      <c r="L53" s="44"/>
-      <c r="M53" s="44"/>
-      <c r="N53" s="44"/>
-      <c r="O53" s="44"/>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B54" s="43"/>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F54" s="44"/>
       <c r="G54" s="44"/>
       <c r="H54" s="44"/>
@@ -2487,25 +2695,12 @@
       <c r="N54" s="44"/>
       <c r="O54" s="44"/>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B55" s="43"/>
       <c r="C55" s="43"/>
       <c r="D55" s="43"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="44"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="44"/>
-      <c r="L55" s="44"/>
-      <c r="M55" s="44"/>
-      <c r="N55" s="44"/>
-      <c r="O55" s="44"/>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B56" s="43"/>
-      <c r="C56" s="43"/>
-      <c r="D56" s="43"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F56" s="44"/>
       <c r="G56" s="44"/>
       <c r="H56" s="44"/>
@@ -2517,22 +2712,27 @@
       <c r="N56" s="44"/>
       <c r="O56" s="44"/>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B57" s="43"/>
       <c r="C57" s="43"/>
       <c r="D57" s="43"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="44"/>
-      <c r="L57" s="44"/>
-      <c r="M57" s="44"/>
-      <c r="N57" s="44"/>
-      <c r="O57" s="44"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B58" s="43"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="44"/>
+      <c r="M58" s="44"/>
+      <c r="N58" s="44"/>
+      <c r="O58" s="44"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B59" s="43"/>
       <c r="C59" s="43"/>
       <c r="D59" s="43"/>
@@ -2547,7 +2747,22 @@
       <c r="N59" s="44"/>
       <c r="O59" s="44"/>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B60" s="43"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="44"/>
+      <c r="M60" s="44"/>
+      <c r="N60" s="44"/>
+      <c r="O60" s="44"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B61" s="43"/>
       <c r="C61" s="43"/>
       <c r="D61" s="43"/>
@@ -2562,10 +2777,7 @@
       <c r="N61" s="44"/>
       <c r="O61" s="44"/>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B62" s="43"/>
-      <c r="C62" s="43"/>
-      <c r="D62" s="43"/>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F62" s="44"/>
       <c r="G62" s="44"/>
       <c r="H62" s="44"/>
@@ -2577,25 +2789,12 @@
       <c r="N62" s="44"/>
       <c r="O62" s="44"/>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B63" s="43"/>
       <c r="C63" s="43"/>
       <c r="D63" s="43"/>
-      <c r="F63" s="44"/>
-      <c r="G63" s="44"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="44"/>
-      <c r="J63" s="44"/>
-      <c r="K63" s="44"/>
-      <c r="L63" s="44"/>
-      <c r="M63" s="44"/>
-      <c r="N63" s="44"/>
-      <c r="O63" s="44"/>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B64" s="43"/>
-      <c r="C64" s="43"/>
-      <c r="D64" s="43"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F64" s="44"/>
       <c r="G64" s="44"/>
       <c r="H64" s="44"/>
@@ -2611,16 +2810,6 @@
       <c r="B65" s="43"/>
       <c r="C65" s="43"/>
       <c r="D65" s="43"/>
-      <c r="F65" s="44"/>
-      <c r="G65" s="44"/>
-      <c r="H65" s="44"/>
-      <c r="I65" s="44"/>
-      <c r="J65" s="44"/>
-      <c r="K65" s="44"/>
-      <c r="L65" s="44"/>
-      <c r="M65" s="44"/>
-      <c r="N65" s="44"/>
-      <c r="O65" s="44"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B66" s="43"/>
@@ -2697,6 +2886,78 @@
       <c r="N70" s="44"/>
       <c r="O70" s="44"/>
     </row>
+    <row r="71" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B71" s="43"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="44"/>
+      <c r="I71" s="44"/>
+      <c r="J71" s="44"/>
+      <c r="K71" s="44"/>
+      <c r="L71" s="44"/>
+      <c r="M71" s="44"/>
+      <c r="N71" s="44"/>
+      <c r="O71" s="44"/>
+    </row>
+    <row r="72" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B72" s="43"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="44"/>
+      <c r="J72" s="44"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="44"/>
+      <c r="N72" s="44"/>
+      <c r="O72" s="44"/>
+    </row>
+    <row r="73" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="44"/>
+      <c r="L73" s="44"/>
+      <c r="M73" s="44"/>
+      <c r="N73" s="44"/>
+      <c r="O73" s="44"/>
+    </row>
+    <row r="74" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="44"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="44"/>
+      <c r="M74" s="44"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="44"/>
+    </row>
+    <row r="75" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="44"/>
+      <c r="J75" s="44"/>
+      <c r="K75" s="44"/>
+      <c r="L75" s="44"/>
+      <c r="M75" s="44"/>
+      <c r="N75" s="44"/>
+      <c r="O75" s="44"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:G1"/>
@@ -2706,15 +2967,15 @@
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="K9:L9"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="F41:M41"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="F46:M46"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J42:K42"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="96" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2733,17 +2994,17 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2751,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2759,10 +3020,10 @@
         <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,10 +3031,10 @@
         <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2791,10 +3052,10 @@
         <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2802,10 +3063,10 @@
         <v>76</v>
       </c>
       <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
         <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2813,10 +3074,10 @@
         <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2824,10 +3085,10 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2835,10 +3096,10 @@
         <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2846,10 +3107,10 @@
         <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2867,7 +3128,7 @@
         <v>100</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3083,8 +3344,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F18C333-41DD-4AE5-A5E3-DF6F4E4DF526}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ac7999f6-dd20-429f-9c50-d27a0c8de317"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>